<commit_message>
Changes in lookup tables
</commit_message>
<xml_diff>
--- a/Input_data/Lookup table - preferred parameter units.xlsx
+++ b/Input_data/Lookup table - preferred parameter units.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DHJ\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC3A6052-90A1-46EA-ACC3-DE0189A0E5F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7068D183-998E-4C27-9D1B-C20A80034CAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="576" yWindow="1008" windowWidth="22224" windowHeight="9756" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="462">
   <si>
     <t>PARAM</t>
   </si>
@@ -1404,6 +1404,9 @@
   </si>
   <si>
     <t>MPHT</t>
+  </si>
+  <si>
+    <t>NG_P_G</t>
   </si>
 </sst>
 </file>
@@ -1739,8 +1742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B448"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A424" workbookViewId="0">
-      <selection activeCell="B448" sqref="B448"/>
+    <sheetView topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A304" sqref="A304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2419,6 +2422,9 @@
       <c r="A85" t="s">
         <v>90</v>
       </c>
+      <c r="B85" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
@@ -5278,10 +5284,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B631D2-CB95-4EE3-9E1E-1DF3BF0D37AD}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5335,6 +5341,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>